<commit_message>
Finish class clust adaptation to arbitrary class nr.s
</commit_message>
<xml_diff>
--- a/Formula Concept Retrieval/diff_eqns_examples/ten examples/diff_eqns2.xlsx
+++ b/Formula Concept Retrieval/diff_eqns_examples/ten examples/diff_eqns2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\Meine Ablage (philippscharpfresearch@gmail.com)\PhD\Projects\Formula Concepts\formula-concept-retrieval\Formula Concept Retrieval\diff_eqns_examples\ten examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD38732C-54C6-419F-AE6E-63E749314C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2213A50B-FA80-4A21-8451-9DAA710E93EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{33029E77-4FD2-4263-950E-5CB3A47A45F4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="202">
   <si>
     <t>\frac{1}{c^2} \frac{\partial^2 \psi}{\partial t^2} - \nabla^2 \psi + \left( \frac{m_0 c}{\hbar} \right)^2 \psi = 0</t>
   </si>
@@ -337,15 +337,9 @@
     <t>\mathbf{E}(\mathbf{r}) = \frac{Q}{4\pi \varepsilon_0} \frac{\hat{\mathbf{r}}}{r^2}</t>
   </si>
   <si>
-    <t>c: "speed of light" (Q2111), \partial: "partial derivative" (Q186475), \psi: "wave function" (Q2362761), t: "time" (Q11471), \nabla: "del" (Q334508), m: "mass" (Q11423) , \hbar: "Planck constant" (Q122894)</t>
-  </si>
-  <si>
     <t>u: "wave function" (Q2362761), t: "time" (Q11471), A: "matrix" (Q44337), f: "function" (Q11348)</t>
   </si>
   <si>
-    <t>\partial: "partial derivative" (Q186475), c: "speed of light" (Q2111), t: "time" (Q11471), h: "wave function" (Q2362761), n: "quantum number" (Q232431), z: "coordinate" (Q12753000), \nu: "frequency" (Q11652)</t>
-  </si>
-  <si>
     <t>\nabla: "del" (Q334508), a: "index number" (Q1738991), \psi: "wave function" (Q2362761), \mu: "mathematical constant" (Q186509)</t>
   </si>
   <si>
@@ -358,12 +352,6 @@
     <t>u: "wave function" (Q2362761), t: "time" (Q11471), \Delta: "Laplace operator" (Q203484), m: "mass" (Q11423)</t>
   </si>
   <si>
-    <t>\eta: "metric tensor" (Q2045231), \mu: "index number" (Q1738991), \nu: "index number" (Q1738991), \partial: "partial derivative" (Q186475), x: "coordinate" (Q12753000), m: "mass" (Q11423), c: "speed of light" (Q2111), \hbar: "Planck constant" (Q122894), \varphi: "wave function" (Q2362761)</t>
-  </si>
-  <si>
-    <t>c: "speed of light" (Q2111), \partial: "partial derivative" (Q186475), t: "time" (Q11471), \sum: "sum" (Q218005), i: "index number" (Q1738991), p: "dimensions" (Q12370773), x: "coordinate" (Q12753000), m: "mass" (Q11423), \hbar: "Planck constant" (Q122894), \varphi: "wave function" (Q2362761)</t>
-  </si>
-  <si>
     <t>G: "Einstein tensor" (Q550929), \mu: "index number" (Q1738991), \nu: "index number" (Q1738991), \Lambda: "cosmological constant" (Q59151), g: "metric tensor" (Q2045231), \kappa: "mathematical constant" (Q186509), T: "stress–energy tensor" (Q876346)</t>
   </si>
   <si>
@@ -388,15 +376,9 @@
     <t>R: "Ricci curvature" (Q1195879), \mu: "index number" (Q1738991), \nu: "index number" (Q1738991), g: "metric tensor" (Q2045231), \Lambda: "cosmological constant" (Q59151), \pi: "mathematical constant" (Q186509), G: "gravitational constant" (Q18373), T: "stress–energy tensor" (Q876346)</t>
   </si>
   <si>
-    <t>R: "Ricci curvature" (Q1195879), \mu: "index number" (Q1738991), \nu: "index number" (Q1738991), g: "metric tensor" (Q2045231), \pi: "mathematical constant" (Q186509), G: "gravitational constant", T: "stress–energy tensor" (Q876346), \Lambda: "cosmological constant" (Q59151)</t>
-  </si>
-  <si>
     <t>div: "divergence" (Q189000), \vec: "vector" (Q13471665), E: "electric field" (Q46221), \pi: "mathematical constant" (Q186509), \rho: "charge density" (Q744771)</t>
   </si>
   <si>
-    <t>\oiint: "surface integral" (Q598146), \partial: "partial derivative" (Q186475), \Omega: "volume element" (Q2327764), E: "electric field" (Q46221), d: "derivative" (Q29175), S: "area" (Q11500), \varepsilon, \iiint: "volume integral" (Q1788036), \rho: "charge density" (Q744771), V volume (Q39297)</t>
-  </si>
-  <si>
     <t>div: "divergence" (Q189000), \vec: "vector" (Q13471665), B: "magnetic field" (Q11408)</t>
   </si>
   <si>
@@ -451,199 +433,214 @@
     <t>CL</t>
   </si>
   <si>
-    <t>\nabla: "del" (Q334508), k: "?" (Q?), A: "matrix" (Q44337), f: "function" (Q11348)</t>
-  </si>
-  <si>
-    <t>\nabla: "del" (Q334508), f: "function" (Q11348), k: "?" (Q?)</t>
-  </si>
-  <si>
-    <t>d: "derivative" (Q29175), T: "stress–energy tensor" (Q876346), t: "time" (Q11471), \omega: "?" (Q?)</t>
-  </si>
-  <si>
-    <t>\nabla: "del" (Q334508), A: "matrix" (Q44337), k: "?" (Q?)</t>
-  </si>
-  <si>
-    <t>\nabla: "del" (Q334508), A: "matrix" (Q44337), i: "index number" (Q1738991), k: "?" (Q?), z: "coordinate" (Q12753000)</t>
-  </si>
-  <si>
-    <t>\nabla: "del" (Q334508), A: "matrix" (Q44337), x: "coordinate" (Q12753000), k: "?" (Q?), f: "function" (Q11348)</t>
-  </si>
-  <si>
-    <t>\nabla: "del" (Q334508), u: "wave function" (Q2362761), k: "?" (Q?)</t>
-  </si>
-  <si>
-    <t>\partial: "partial derivative" (Q186475), u: "wave function" (Q2362761), x: "coordinate" (Q12753000), y: "?" (Q?), z: "coordinate" (Q12753000), k: "?" (Q?)</t>
-  </si>
-  <si>
-    <t>\nabla: "del" (Q334508), u: "wave function" (Q2362761), k: "?" (Q?), \rho: "charge density" (Q744771), \psi: "wave function" (Q2362761)</t>
-  </si>
-  <si>
-    <t>\nabla: "del" (Q334508), u: "wave function" (Q2362761), k: "?" (Q?), \rho: "charge density" (Q744771), \psi: "wave function" (Q2362761), z: "coordinate" (Q12753000), \partial: "partial derivative" (Q186475), \phi: "wave function" (Q2362761)</t>
-  </si>
-  <si>
-    <t>\nabla: "del" (Q334508), \varphi: "wave function" (Q2362761)</t>
-  </si>
-  <si>
-    <t>\Delta: "Laplace operator" (Q203484), \varphi: "wave function" (Q2362761)</t>
-  </si>
-  <si>
-    <t>i: "index number" (Q1738991), n: "quantum number" (Q232431), j: "four-current" (Q2074152), partial: "?" (Q?), \varphi: "wave function" (Q2362761)</t>
-  </si>
-  <si>
-    <t>i: "index number" (Q1738991), n: "quantum number" (Q232431), \partial: "partial derivative" (Q186475), j: "four-current" (Q2074152)</t>
-  </si>
-  <si>
-    <t>\partial: "partial derivative" (Q186475), \varphi: "wave function" (Q2362761), x: "coordinate" (Q12753000), y: "?" (Q?), z: "coordinate" (Q12753000)</t>
-  </si>
-  <si>
-    <t>r: "critical radius" (Q4241349), \partial: "partial derivative" (Q186475), \varphi: "wave function" (Q2362761), \theta: "?" (Q?)</t>
-  </si>
-  <si>
-    <t>\Delta: "Laplace operator" (Q203484), u: "wave function" (Q2362761), x: "coordinate" (Q12753000), y: "?" (Q?)</t>
-  </si>
-  <si>
-    <t>\Delta: "Laplace operator" (Q203484), u: "wave function" (Q2362761), x: "coordinate" (Q12753000), y: "?" (Q?), f: "function" (Q11348)</t>
-  </si>
-  <si>
-    <t>\phi: "wave function" (Q2362761), r: "critical radius" (Q4241349)</t>
-  </si>
-  <si>
-    <t>\vec: "vector" (Q13471665), F: "electromagnetic field" (Q177625), p: "dimensions" (Q12370773), d: "derivative" (Q29175), t: "time" (Q11471)</t>
-  </si>
-  <si>
-    <t>\vec: "vector" (Q13471665), F: "electromagnetic field" (Q177625), m: "mass" (Q11423), a: "mathematical constant" (Q186509)</t>
-  </si>
-  <si>
-    <t>\vec: "vector" (Q13471665), F: "electromagnetic field" (Q177625), m: "mass" (Q11423), d: "derivative" (Q29175), t: "time" (Q11471), s: "?" (Q?)</t>
-  </si>
-  <si>
-    <t>F: "electromagnetic field" (Q177625), d: "derivative" (Q29175), t: "time" (Q11471), m: "mass" (Q11423), v: "?" (Q?)</t>
-  </si>
-  <si>
-    <t>\vec: "vector" (Q13471665), F: "electromagnetic field" (Q177625), \Delta: "Laplace operator" (Q203484), p: "dimensions" (Q12370773)</t>
-  </si>
-  <si>
-    <t>\vec: "vector" (Q13471665), F: "electromagnetic field" (Q177625), m: "mass" (Q11423), \Delta: "Laplace operator" (Q203484), v: "?" (Q?), t: "time" (Q11471)</t>
-  </si>
-  <si>
-    <t>\vec: "vector" (Q13471665), F: "electromagnetic field" (Q177625), p: "dimensions" (Q12370773), t: "time" (Q11471)</t>
-  </si>
-  <si>
-    <t>F: "electromagnetic field" (Q177625), m: "mass" (Q11423), a: "mathematical constant" (Q186509)</t>
-  </si>
-  <si>
-    <t>F: "electromagnetic field" (Q177625), k: "?" (Q?), m: "mass" (Q11423), a: "mathematical constant" (Q186509)</t>
-  </si>
-  <si>
-    <t>\sigma: "?" (Q?), x: "coordinate" (Q12753000), p: "dimensions" (Q12370773), \hbar: "Planck constant" (Q122894)</t>
-  </si>
-  <si>
-    <t>\sigma: "?" (Q?), E: "electric field" (Q46221), B: "magnetic field" (Q11408), d: "derivative" (Q29175), t: "time" (Q11471), \hbar: "Planck constant" (Q122894)</t>
-  </si>
-  <si>
-    <t>\sigma: "?" (Q?), J: "?" (Q?), x: "coordinate" (Q12753000), y: "?" (Q?), z: "coordinate" (Q12753000), j: "four-current" (Q2074152)</t>
-  </si>
-  <si>
-    <t>\Delta: "Laplace operator" (Q203484), x: "coordinate" (Q12753000), p: "dimensions" (Q12370773), \hbar: "Planck constant" (Q122894)</t>
-  </si>
-  <si>
-    <t>\sigma: "?" (Q?), x: "coordinate" (Q12753000), p: "dimensions" (Q12370773), i: "index number" (Q1738991), \vec: "vector" (Q13471665)</t>
-  </si>
-  <si>
-    <t>\sigma: "?" (Q?), x: "coordinate" (Q12753000), p: "dimensions" (Q12370773), A: "matrix" (Q44337), B: "magnetic field" (Q11408)</t>
-  </si>
-  <si>
-    <t>\sigma: "?" (Q?), x: "coordinate" (Q12753000), p: "dimensions" (Q12370773), \hbar: "Planck constant" (Q122894), \Psi: "wave function" (Q2362761), d: "derivative" (Q29175)</t>
-  </si>
-  <si>
-    <t>\sigma: "?" (Q?), x: "coordinate" (Q12753000), p: "dimensions" (Q12370773), i: "index number" (Q1738991), \hbar: "Planck constant" (Q122894)</t>
-  </si>
-  <si>
-    <t>\sigma: "?" (Q?), x: "coordinate" (Q12753000), p: "dimensions" (Q12370773), \int \Psi: "?" (Q?), d: "derivative" (Q29175)</t>
-  </si>
-  <si>
-    <t>\oint: "line integral" (Q467699), \delta: "natural number" (Q21199), Q: "?" (Q?), T: "stress–energy tensor" (Q876346)</t>
-  </si>
-  <si>
-    <t>\Delta: "Laplace operator" (Q203484), S: "area" (Q11500), \int: "?" (Q?), \delta: "natural number" (Q21199), Q: "?" (Q?), T: "stress–energy tensor" (Q876346)</t>
-  </si>
-  <si>
-    <t>d: "derivative" (Q29175), S: "area" (Q11500), R: "Ricci curvature" (Q1195879)</t>
-  </si>
-  <si>
-    <t>S: "area" (Q11500)</t>
-  </si>
-  <si>
-    <t>d: "derivative" (Q29175), E: "electric field" (Q46221), \delta: "natural number" (Q21199), w: "?" (Q?), u: "wave function" (Q2362761)</t>
-  </si>
-  <si>
-    <t>\int: "?" (Q?), \delta: "natural number" (Q21199), Q: "?" (Q?), T: "stress–energy tensor" (Q876346), N: "mathematical constant" (Q186509)</t>
-  </si>
-  <si>
-    <t>d: "derivative" (Q29175), S: "area" (Q11500), t: "time" (Q11471)</t>
-  </si>
-  <si>
-    <t>d: "derivative" (Q29175), S: "area" (Q11500), t: "time" (Q11471), i: "index number" (Q1738991)</t>
-  </si>
-  <si>
-    <t>d: "derivative" (Q29175), S: "area" (Q11500), t: "time" (Q11471), \dot: "?" (Q?), Q: "?" (Q?), T: "stress–energy tensor" (Q876346), i: "index number" (Q1738991)</t>
-  </si>
-  <si>
-    <t>d: "derivative" (Q29175), S: "area" (Q11500), \delta: "natural number" (Q21199), Q: "?" (Q?), T: "stress–energy tensor" (Q876346)</t>
-  </si>
-  <si>
-    <t>F: "electromagnetic field" (Q177625), q: "?" (Q?), \times: "?" (Q?), r: "critical radius" (Q4241349)</t>
-  </si>
-  <si>
-    <t>F: "electromagnetic field" (Q177625), k: "?" (Q?), e: "?" (Q?), q: "?" (Q?), r: "critical radius" (Q4241349)</t>
-  </si>
-  <si>
-    <t>F: "electromagnetic field" (Q177625), q: "?" (Q?), \varepsilon: "Levi-Civita symbol" (Q623761), r: "critical radius" (Q4241349)</t>
-  </si>
-  <si>
-    <t>F: "electromagnetic field" (Q177625), r: "critical radius" (Q4241349), q: "?" (Q?), \varepsilon: "Levi-Civita symbol" (Q623761), i: "index number" (Q1738991), N: "mathematical constant" (Q186509)</t>
-  </si>
-  <si>
-    <t>F: "electromagnetic field" (Q177625), r: "critical radius" (Q4241349), q: "?" (Q?), \varepsilon: "Levi-Civita symbol" (Q623761), i: "index number" (Q1738991), N: "mathematical constant" (Q186509), R: "Ricci curvature" (Q1195879)</t>
-  </si>
-  <si>
-    <t>F: "electromagnetic field" (Q177625), r: "critical radius" (Q4241349), q: "?" (Q?), \varepsilon: "Levi-Civita symbol" (Q623761), \int: "?" (Q?), d: "derivative" (Q29175)</t>
-  </si>
-  <si>
-    <t>E: "electric field" (Q46221), r: "critical radius" (Q4241349), \varepsilon: "Levi-Civita symbol" (Q623761), i: "index number" (Q1738991), N: "mathematical constant" (Q186509), q: "?" (Q?)</t>
-  </si>
-  <si>
-    <t>E: "electric field" (Q46221), r: "critical radius" (Q4241349), Q: "?" (Q?), \varepsilon: "Levi-Civita symbol" (Q623761)</t>
-  </si>
-  <si>
-    <t>i: " complex number" (Q11567), \hbar: "Planck constant" (Q122894), \partial: "partial derivative" (Q186475), t: "time" (Q11471), \Psi: "wave function" (Q2362761), x: "coordinate" (Q12753000), m: "mass" (Q11423), V: "potential energy" (Q155640)</t>
-  </si>
-  <si>
-    <t>i: " complex number" (Q11567), \hbar: "Planck constant" (Q122894), \partial: "partial derivative" (Q186475), t: "time" (Q11471), \psi: "wave function" (Q2362761), H: "Hamiltonian operator" (Q660488)</t>
-  </si>
-  <si>
-    <t>i: " complex number" (Q11567), \hbar: "Planck constant" (Q122894), d: "derivative" (Q29175), t: "time" (Q11471), Psi: "wave function" (Q2362761), H: "Hamiltonian operator" (Q660488)</t>
-  </si>
-  <si>
-    <t>i: " complex number" (Q11567), \hbar: "Planck constant" (Q122894), d: "derivative" (Q29175), \Psi: "wave function" (Q2362761), t: "time" (Q11471), m: "mass" (Q11423), p: "momentum" (Q41273), V: "potential energy" (Q155640)</t>
-  </si>
-  <si>
-    <t>i: " complex number" (Q11567), \hbar: "Planck constant" (Q122894), \partial: "partial derivative" (Q186475), t: "time" (Q11471), \Psi: "wave function" (Q2362761), r: "distance" (Q126017), m: "mass" (Q11423), \nabla: "del" (Q334508), V: "potential energy" (Q155640)</t>
-  </si>
-  <si>
     <t>H: "Hamiltonian operator" (Q660488), \Psi: "wave function" (Q2362761), E: "energy" (Q11379)</t>
   </si>
   <si>
-    <t>\hbar: "Planck constant" (Q122894), m: "mass" (Q11423), d: "derivative" (Q29175), \psi: "wave function" (Q2362761), x: "coordinate" (Q12753000), E: "energy" (Q11379)</t>
-  </si>
-  <si>
-    <t>E: "energy" (Q11379), \psi: "wave function" (Q2362761), \hbar: "Planck constant" (Q122894), m: "mass" (Q11423), d: "derivative" (Q29175), x: "coordinate" (Q12753000), \omega: " angular velocity" (Q161635)</t>
-  </si>
-  <si>
-    <t>E: "energy" (Q11379), \psi: "wave function" (Q2362761), \hbar: "Planck constant" (Q122894), \mu: "mass" (Q11423)  (Q1515261), \nabla: "del" (Q334508), q: "electric charge" (Q1111), \varepsilon: "vacuum permittivity" (Q6158) , r: "distance" (Q126017)</t>
-  </si>
-  <si>
-    <t>i: " complex number" (Q11567), \hbar: "Planck constant" (Q122894), \partial: "partial derivative" (Q186475), t: "time" (Q11471), \Psi: "wave function" (Q2362761), r: "distance" (Q126017), H: "Hamiltonian operator" (Q660488)</t>
+    <t>d: "derivative" (Q29175), T: "scalar function" (Q91108373), t: "time" (Q11471), \omega:  "angular frequency" (Q834020)</t>
+  </si>
+  <si>
+    <t>i: "complex number" (Q11567), \hbar: "Planck constant" (Q122894), \partial: "partial derivative" (Q186475), t: "time" (Q11471), \Psi: "wave function" (Q2362761), r: "distance" (Q126017), H: "Hamiltonian operator" (Q660488)</t>
+  </si>
+  <si>
+    <t>i: "complex number" (Q11567), \hbar: "Planck constant" (Q122894), \partial: "partial derivative" (Q186475), t: "time" (Q11471), \Psi: "wave function" (Q2362761), r: "distance" (Q126017), m: "mass" (Q11423), \nabla: "del" (Q334508), V: "potential energy" (Q155640)</t>
+  </si>
+  <si>
+    <t>i: "complex number" (Q11567), \hbar: "Planck constant" (Q122894), d: "derivative" (Q29175), \Psi: "wave function" (Q2362761), t: "time" (Q11471), m: "mass" (Q11423), p: "momentum" (Q41273), V: "potential energy" (Q155640)</t>
+  </si>
+  <si>
+    <t>i: "complex number" (Q11567), \hbar: "Planck constant" (Q122894), d: "derivative" (Q29175), t: "time" (Q11471), Psi: "wave function" (Q2362761), H: "Hamiltonian operator" (Q660488)</t>
+  </si>
+  <si>
+    <t>i: "complex number" (Q11567), \hbar: "Planck constant" (Q122894), \partial: "partial derivative" (Q186475), t: "time" (Q11471), \psi: "wave function" (Q2362761), H: "Hamiltonian operator" (Q660488)</t>
+  </si>
+  <si>
+    <t>\nabla: "del" (Q334508), f: "eigenfunction" (Q1307821), k: "eigenvalue" (Q3553768)</t>
+  </si>
+  <si>
+    <t>\nabla: "del" (Q334508), \varphi: "scalar function" (Q91108373)</t>
+  </si>
+  <si>
+    <t>\Delta: "Laplace operator" (Q203484), \varphi: "scalar function" (Q91108373)</t>
+  </si>
+  <si>
+    <t>i: "index number" (Q1738991), n: "dimension" (Q4440864), \partial: "partial derivative" (Q186475), j: "index number" (Q1738991), \varphi: "scalar function" (Q91108373)</t>
+  </si>
+  <si>
+    <t>\partial: "partial derivative" (Q186475), c: "speed of light" (Q2111), t: "time" (Q11471), h: "wave function" (Q2362761), n: "quantum number" (Q232431), z: "coordinate" (Q3250736), \nu: "frequency" (Q11652)</t>
+  </si>
+  <si>
+    <t>\eta: "metric tensor" (Q2045231), \mu: "index number" (Q1738991), \nu: "index number" (Q1738991), \partial: "partial derivative" (Q186475), x: "coordinate" (Q3250736), m: "mass" (Q11423), c: "speed of light" (Q2111), \hbar: "Planck constant" (Q122894), \varphi: "wave function" (Q2362761)</t>
+  </si>
+  <si>
+    <t>c: "speed of light" (Q2111), \partial: "partial derivative" (Q186475), t: "time" (Q11471), \sum: "sum" (Q218005), i: "index number" (Q1738991), p: "dimensions" (Q12370773), x: "coordinate" (Q3250736), m: "mass" (Q11423), \hbar: "Planck constant" (Q122894), \varphi: "wave function" (Q2362761)</t>
+  </si>
+  <si>
+    <t>i: "complex number" (Q11567), \hbar: "Planck constant" (Q122894), \partial: "partial derivative" (Q186475), t: "time" (Q11471), \Psi: "wave function" (Q2362761), x: "coordinate" (Q3250736), m: "mass" (Q11423), V: "potential energy" (Q155640)</t>
+  </si>
+  <si>
+    <t>\hbar: "Planck constant" (Q122894), m: "mass" (Q11423), d: "derivative" (Q29175), \psi: "wave function" (Q2362761), x: "coordinate" (Q3250736), E: "energy" (Q11379)</t>
+  </si>
+  <si>
+    <t>E: "energy" (Q11379), \psi: "wave function" (Q2362761), \hbar: "Planck constant" (Q122894), m: "mass" (Q11423), d: "derivative" (Q29175), x: "coordinate" (Q3250736), \omega: " angular velocity" (Q161635)</t>
+  </si>
+  <si>
+    <t>\nabla: "del" (Q334508), f: "eigenfunction" (Q1307821), i: "complex number" (Q11567), k: "eigenvalue" (Q3553768), z: "coordinate" (Q3250736)</t>
+  </si>
+  <si>
+    <t>\nabla: "del" (Q334508), A: "scalar function" (Q91108373), x: "coordinate" (Q3250736), k: "eigenvalue" (Q3553768), f: "function" (Q11348)</t>
+  </si>
+  <si>
+    <t>\nabla: "del" (Q334508), u: "wave function" (Q2362761), k: "wavenumber" (Q192510), \rho: "coordinate" (Q3250736), \psi: "coordinate" (Q3250736)</t>
+  </si>
+  <si>
+    <t>\partial: "partial derivative" (Q186475), \varphi: "scalar function" (Q91108373), x: "coordinate" (Q3250736), y: "coordinate" (Q3250736), z: "coordinate" (Q3250736)</t>
+  </si>
+  <si>
+    <t>r: "coordinate" (Q3250736), \partial: "partial derivative" (Q186475), \varphi: "scalar function" (Q91108373), \theta: "coordinate" (Q3250736)</t>
+  </si>
+  <si>
+    <t>\Delta: "Laplace operator" (Q203484), u: "scalar function" (Q91108373), x: "coordinate" (Q3250736), y: "coordinate" (Q3250736), f: "scalar function" (Q91108373)</t>
+  </si>
+  <si>
+    <t>\phi: "scalar function" (Q91108373), r: "coordinate" (Q3250736)</t>
+  </si>
+  <si>
+    <t>\vec: "vector" (Q13471665), F: "force" (Q11402), m: "mass" (Q11423), \Delta: "difference" (Q29896155), v: "velocity" (Q11465), t: "time" (Q11471)</t>
+  </si>
+  <si>
+    <t>F: "force" (Q11402), \propto: "proportionality" (Q51379), m: "mass" (Q11423), a:  "acceleration" (Q11376)</t>
+  </si>
+  <si>
+    <t>\vec: "vector" (Q13471665), F: "force" (Q11402), p: "momentum" (Q41273), d: "derivative" (Q29175), t: "time" (Q11471)</t>
+  </si>
+  <si>
+    <t>\vec: "vector" (Q13471665), F: "force" (Q11402), m: "mass" (Q11423), a:  "acceleration" (Q11376)</t>
+  </si>
+  <si>
+    <t>\vec: "vector" (Q13471665), F: "force" (Q11402), m: "mass" (Q11423), d: "derivative" (Q29175), t: "time" (Q11471), s: "coordinate" (Q3250736)</t>
+  </si>
+  <si>
+    <t>F: "force" (Q11402), d: "derivative" (Q29175), t: "time" (Q11471), m: "mass" (Q11423), v: "velocity" (Q11465)</t>
+  </si>
+  <si>
+    <t>\vec: "vector" (Q13471665), F: "force" (Q11402), \Delta: "difference" (Q29896155), p: "momentum" (Q41273)</t>
+  </si>
+  <si>
+    <t>\vec: "vector" (Q13471665), F: "force" (Q11402), p: "momentum" (Q41273), t: "time" (Q11471)</t>
+  </si>
+  <si>
+    <t>\sigma: "uncertainty" (Q13649246), E: "electric field" (Q46221), B: "magnetic field" (Q11408), d: "derivative" (Q29175), t: "time" (Q11471), \hbar: "Planck constant" (Q122894)</t>
+  </si>
+  <si>
+    <t>\sigma: "uncertainty" (Q13649246), x: "coordinate" (Q3250736), p: "momentum" (Q41273), \hbar: "Planck constant" (Q122894)</t>
+  </si>
+  <si>
+    <t>\Delta: "uncertainty" (Q13649246), x: "coordinate" (Q3250736), p: "momentum" (Q41273), \hbar: "Planck constant" (Q122894)</t>
+  </si>
+  <si>
+    <t>\sigma: "uncertainty" (Q13649246), x: "coordinate" (Q3250736), p: "momentum" (Q41273), i: "complex number" (Q11567), \vec: "vector" (Q13471665)</t>
+  </si>
+  <si>
+    <t>\sigma: "uncertainty" (Q13649246), x: "coordinate" (Q3250736), p: "momentum" (Q41273), \hbar: "Planck constant" (Q122894), \Psi: "wave function" (Q2362761), d: "derivative" (Q29175)</t>
+  </si>
+  <si>
+    <t>\nabla: "del" (Q334508), u: "wave function" (Q2362761), k: "wavenumber" (Q192510), \rho: "coordinate" (Q3250736), \psi: "coordinate" (Q3250736), z: "coordinate" (Q3250736), \partial: "partial derivative" (Q186475), \phi: "coordinate" (Q3250736)</t>
+  </si>
+  <si>
+    <t>\sigma: "uncertainty" (Q13649246), x: "coordinate" (Q3250736), p: "momentum" (Q41273), A: "matrix" (Q44337), B: "matrix" (Q44337)</t>
+  </si>
+  <si>
+    <t>\sigma: "uncertainty" (Q13649246), x: "coordinate" (Q3250736), p: "momentum" (Q41273), i: "complex number" (Q11567), \hbar: "Planck constant" (Q122894)</t>
+  </si>
+  <si>
+    <t>E: "electric field" (Q46221), r: "coordinate" (Q3250736), Q: "electric charge" (Q1111), \varepsilon: "vacuum permittivity" (Q6158)</t>
+  </si>
+  <si>
+    <t>F: "force" (Q11402), q: "electric charge" (Q1111), \varepsilon: "vacuum permittivity" (Q6158), r: "distance" (Q126017)</t>
+  </si>
+  <si>
+    <t>\oiint: "surface integral" (Q598146), \partial: "partial derivative" (Q186475), \Omega: "volume element" (Q2327764), E: "electric field" (Q46221), d: "derivative" (Q29175), S: "area" (Q11500), \varepsilon: "vacuum permittivity" (Q6158), \iiint: "volume integral" (Q1788036), \rho: "charge density" (Q744771), V: volume (Q39297)</t>
+  </si>
+  <si>
+    <t>\Delta: "Laplace operator" (Q203484), u: "scalar function" (Q91108373), x: "coordinate" (Q3250736), y: "coordinate" (Q3250736)</t>
+  </si>
+  <si>
+    <t>c: "speed of light" (Q2111), \partial: "partial derivative" (Q186475), \psi: "wave function" (Q2362761), t: "time" (Q11471), \nabla: "del" (Q334508), m: "mass" (Q11423), \hbar: "Planck constant" (Q122894)</t>
+  </si>
+  <si>
+    <t>E: "energy" (Q11379), \psi: "wave function" (Q2362761), \hbar: "Planck constant" (Q122894), \mu: "mass" (Q11423), \nabla: "del" (Q334508), q: "electric charge" (Q1111), \varepsilon: "vacuum permittivity" (Q6158), r: "distance" (Q126017)</t>
+  </si>
+  <si>
+    <t>R: "Ricci curvature" (Q1195879), \mu: "index number" (Q1738991), \nu: "index number" (Q1738991), g: "metric tensor" (Q2045231), \pi: "mathematical constant" (Q186509), G: "gravitational constant" (Q18373), T: "stress–energy tensor" (Q876346), \Lambda: "cosmological constant" (Q59151)</t>
+  </si>
+  <si>
+    <t>\sigma: "uncertainty" (Q13649246), J: "angular momentum" (Q161254), x: "coordinate" (Q3250736), y: "coordinate" (Q3250736), z: "coordinate" (Q3250736), j: "angular momentum" (Q161254)</t>
+  </si>
+  <si>
+    <t>\sigma: "uncertainty" (Q13649246), x: "coordinate" (Q3250736), p: "momentum" (Q41273), \int: "integral" (Q80091), \Psi: "wave function" (Q2362761), d: "derivative" (Q29175)</t>
+  </si>
+  <si>
+    <t>F: "force" (Q11402), r: "coordinate" (Q3250736), q: "electric charge" (Q1111), \varepsilon: "vacuum permittivity" (Q6158), \int: "integral" (Q80091), d: "derivative" (Q29175)</t>
+  </si>
+  <si>
+    <t>S: "entropy" (Q45003)</t>
+  </si>
+  <si>
+    <t>d: "derivative" (Q29175), S: "entropy" (Q45003), t: "time" (Q11471)</t>
+  </si>
+  <si>
+    <t>d: "derivative" (Q29175), S: "entropy" (Q45003), t: "time" (Q11471), i: "index number" (Q1738991)</t>
+  </si>
+  <si>
+    <t>d: "derivative" (Q29175), S: "entropy" (Q45003), R: "molar gas constant" (Q182333)</t>
+  </si>
+  <si>
+    <t>d: "derivative" (Q29175), E: "energy" (Q11379), \delta: "natural number" (Q21199), w: "work" (Q42213), u: "wave function" (Q2362761)</t>
+  </si>
+  <si>
+    <t>d: "derivative" (Q29175), S: "entropy" (Q45003), t: "time" (Q11471), \dot: "time derivative" (Q6960532), Q: "heat" (Q44432), T: "temperature" (Q11466), i: "index number" (Q1738991)</t>
+  </si>
+  <si>
+    <t>d: "derivative" (Q29175), S: "entropy" (Q45003), \delta: "natural number" (Q21199), Q: "heat" (Q44432), T: "temperature" (Q11466)</t>
+  </si>
+  <si>
+    <t>\oint: "line integral" (Q467699), \delta: "difference" (Q29896155), Q: "heat" (Q44432), T: "temperature" (Q11466)</t>
+  </si>
+  <si>
+    <t>\Delta: "difference" (Q29896155), S: "entropy" (Q45003), \int: "integral" (Q80091), \delta: "difference" (Q29896155), Q: "heat" (Q44432), T: "temperature" (Q11466)</t>
+  </si>
+  <si>
+    <t>\int: "integral" (Q80091), \delta: "natural number" (Q21199), Q: "heat" (Q44432), T: "temperature" (Q11466), N: "entropy" (Q45003)</t>
+  </si>
+  <si>
+    <t>F: "force" (Q11402), q: "electric charge" (Q1111), \times: "vector product" (Q178192), r: "distance" (Q126017)</t>
+  </si>
+  <si>
+    <t>F: "force" (Q11402), k: "mathematical constant" (Q186509), m: "mass" (Q11423), a:  "acceleration" (Q11376)</t>
+  </si>
+  <si>
+    <t>F: "force" (Q11402), k: "mathematical constant" (Q186509), e: "name" (Q82799), q: "electric charge" (Q1111), r: "distance" (Q126017)</t>
+  </si>
+  <si>
+    <t>F: "force" (Q11402), r: "coordinate" (Q3250736), q: "electric charge" (Q1111), \varepsilon: "vacuum permittivity" (Q6158), i: "index number" (Q1738991), N: "number of particles" (Q181155)</t>
+  </si>
+  <si>
+    <t>F: "force" (Q11402), r: "coordinate" (Q3250736), q: "electric charge" (Q1111), \varepsilon: "vacuum permittivity" (Q6158), i: "index number" (Q1738991), N: "number of particles" (Q181155), R: "distance" (Q126017)</t>
+  </si>
+  <si>
+    <t>E: "electric field" (Q46221), r: "coordinate" (Q3250736), \varepsilon: "vacuum permittivity" (Q6158), i: "index number" (Q1738991), N: "number of particles" (Q181155), q: "electric charge" (Q1111)</t>
+  </si>
+  <si>
+    <t>i: "index number" (Q1738991), n: "dimension" (Q4440864), j: "index number" (Q1738991), partial: "partial derivative" (Q186475), \varphi: "scalar function" (Q91108373)</t>
+  </si>
+  <si>
+    <t>\partial: "partial derivative" (Q186475), u: "wave function" (Q2362761), x: "coordinate" (Q3250736), y: "coordinate" (Q3250736), z: "coordinate" (Q3250736), k: "wavenumber" (Q192510)</t>
+  </si>
+  <si>
+    <t>\nabla: "del" (Q334508), u: "wave function" (Q2362761), k: "wavenumber" (Q192510)</t>
+  </si>
+  <si>
+    <t>\nabla: "del" (Q334508), k: "eigenvalue" (Q3553768), A: "scalar function" (Q91108373), f: "eigenfunction" (Q1307821)</t>
   </si>
 </sst>
 </file>
@@ -1005,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0363C22-33ED-4C57-BC4A-196E9CD28EC8}">
   <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1016,1102 +1013,1102 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>108</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>119</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>193</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>195</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>198</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>196</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>197</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>199</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>200</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>202</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B41" t="s">
         <v>40</v>
       </c>
-      <c r="C41" t="s">
-        <v>138</v>
+      <c r="C41" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
-      <c r="C43" t="s">
-        <v>140</v>
+      <c r="C43" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
-      <c r="C44" t="s">
-        <v>141</v>
+      <c r="C44" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B45" t="s">
         <v>44</v>
       </c>
-      <c r="C45" t="s">
-        <v>142</v>
+      <c r="C45" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B46" t="s">
         <v>45</v>
       </c>
-      <c r="C46" t="s">
-        <v>143</v>
+      <c r="C46" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
-      <c r="C47" t="s">
-        <v>144</v>
+      <c r="C47" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
-      <c r="C48" t="s">
-        <v>145</v>
+      <c r="C48" s="1" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
-      <c r="C49" t="s">
-        <v>146</v>
+      <c r="C49" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
       </c>
-      <c r="C50" t="s">
-        <v>147</v>
+      <c r="C50" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
-      <c r="C51" t="s">
-        <v>148</v>
+      <c r="C51" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B52" t="s">
         <v>51</v>
       </c>
-      <c r="C52" t="s">
-        <v>148</v>
+      <c r="C52" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B53" t="s">
         <v>52</v>
       </c>
-      <c r="C53" t="s">
-        <v>149</v>
+      <c r="C53" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B54" t="s">
         <v>53</v>
       </c>
-      <c r="C54" t="s">
-        <v>150</v>
+      <c r="C54" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
       </c>
-      <c r="C55" t="s">
-        <v>151</v>
+      <c r="C55" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B56" t="s">
         <v>55</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B57" t="s">
         <v>56</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="1" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B58" t="s">
         <v>57</v>
       </c>
-      <c r="C58" t="s">
-        <v>154</v>
+      <c r="C58" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B59" t="s">
         <v>58</v>
       </c>
-      <c r="C59" t="s">
-        <v>155</v>
+      <c r="C59" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B60" t="s">
         <v>59</v>
       </c>
-      <c r="C60" t="s">
-        <v>156</v>
+      <c r="C60" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B61" t="s">
         <v>60</v>
       </c>
-      <c r="C61" t="s">
-        <v>157</v>
+      <c r="C61" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B62" t="s">
         <v>61</v>
       </c>
-      <c r="C62" t="s">
-        <v>158</v>
+      <c r="C62" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B63" t="s">
         <v>62</v>
       </c>
-      <c r="C63" t="s">
-        <v>159</v>
+      <c r="C63" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B64" t="s">
         <v>63</v>
       </c>
-      <c r="C64" t="s">
-        <v>160</v>
+      <c r="C64" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B65" t="s">
         <v>64</v>
       </c>
-      <c r="C65" t="s">
-        <v>161</v>
+      <c r="C65" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B66" t="s">
         <v>65</v>
       </c>
-      <c r="C66" t="s">
-        <v>162</v>
+      <c r="C66" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B67" t="s">
         <v>66</v>
       </c>
-      <c r="C67" t="s">
-        <v>162</v>
+      <c r="C67" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B68" t="s">
         <v>67</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="1" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B69" t="s">
         <v>68</v>
       </c>
-      <c r="C69" t="s">
-        <v>164</v>
+      <c r="C69" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B70" t="s">
         <v>69</v>
       </c>
-      <c r="C70" t="s">
-        <v>165</v>
+      <c r="C70" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B71" t="s">
         <v>70</v>
       </c>
-      <c r="C71" t="s">
-        <v>166</v>
+      <c r="C71" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B72" t="s">
         <v>71</v>
       </c>
-      <c r="C72" t="s">
-        <v>167</v>
+      <c r="C72" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B73" t="s">
         <v>72</v>
       </c>
-      <c r="C73" t="s">
-        <v>168</v>
+      <c r="C73" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B74" t="s">
         <v>73</v>
       </c>
-      <c r="C74" t="s">
-        <v>169</v>
+      <c r="C74" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B75" t="s">
         <v>74</v>
       </c>
-      <c r="C75" t="s">
-        <v>170</v>
+      <c r="C75" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B76" t="s">
         <v>75</v>
       </c>
-      <c r="C76" t="s">
-        <v>166</v>
+      <c r="C76" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B77" t="s">
         <v>76</v>
       </c>
-      <c r="C77" t="s">
-        <v>171</v>
+      <c r="C77" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B78" t="s">
         <v>77</v>
       </c>
-      <c r="C78" t="s">
-        <v>172</v>
+      <c r="C78" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B79" t="s">
         <v>78</v>
       </c>
-      <c r="C79" t="s">
-        <v>173</v>
+      <c r="C79" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B80" t="s">
         <v>79</v>
       </c>
-      <c r="C80" t="s">
-        <v>174</v>
+      <c r="C80" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B81" t="s">
         <v>80</v>
       </c>
-      <c r="C81" t="s">
-        <v>175</v>
+      <c r="C81" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B82" t="s">
         <v>81</v>
       </c>
-      <c r="C82" t="s">
-        <v>176</v>
+      <c r="C82" s="1" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B83" t="s">
         <v>82</v>
       </c>
-      <c r="C83" t="s">
-        <v>177</v>
+      <c r="C83" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B84" t="s">
         <v>83</v>
       </c>
-      <c r="C84" t="s">
-        <v>178</v>
+      <c r="C84" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B85" t="s">
         <v>84</v>
       </c>
-      <c r="C85" t="s">
-        <v>179</v>
+      <c r="C85" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B86" t="s">
         <v>85</v>
       </c>
-      <c r="C86" t="s">
-        <v>180</v>
+      <c r="C86" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B87" t="s">
         <v>86</v>
       </c>
-      <c r="C87" t="s">
-        <v>181</v>
+      <c r="C87" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B88" t="s">
         <v>87</v>
       </c>
-      <c r="C88" t="s">
-        <v>182</v>
+      <c r="C88" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B89" t="s">
         <v>88</v>
       </c>
-      <c r="C89" t="s">
-        <v>183</v>
+      <c r="C89" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B90" t="s">
         <v>89</v>
       </c>
-      <c r="C90" t="s">
-        <v>184</v>
+      <c r="C90" s="1" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B91" t="s">
         <v>90</v>
       </c>
-      <c r="C91" t="s">
-        <v>185</v>
+      <c r="C91" s="1" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B92" t="s">
         <v>91</v>
       </c>
-      <c r="C92" t="s">
-        <v>186</v>
+      <c r="C92" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B93" t="s">
         <v>92</v>
       </c>
-      <c r="C93" t="s">
-        <v>186</v>
+      <c r="C93" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B94" t="s">
         <v>93</v>
       </c>
-      <c r="C94" t="s">
-        <v>187</v>
+      <c r="C94" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B95" t="s">
         <v>94</v>
       </c>
-      <c r="C95" t="s">
-        <v>187</v>
+      <c r="C95" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B96" t="s">
         <v>95</v>
       </c>
-      <c r="C96" t="s">
-        <v>188</v>
+      <c r="C96" s="1" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B97" t="s">
         <v>96</v>
       </c>
-      <c r="C97" t="s">
-        <v>189</v>
+      <c r="C97" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B98" t="s">
         <v>97</v>
       </c>
-      <c r="C98" t="s">
-        <v>190</v>
+      <c r="C98" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B99" t="s">
         <v>98</v>
       </c>
-      <c r="C99" t="s">
-        <v>191</v>
+      <c r="C99" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B100" t="s">
         <v>99</v>
       </c>
-      <c r="C100" t="s">
-        <v>192</v>
+      <c r="C100" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>